<commit_message>
Fixed doseQuantity should be array
</commit_message>
<xml_diff>
--- a/OrderSentences_Review.xlsx
+++ b/OrderSentences_Review.xlsx
@@ -4136,7 +4136,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Naseptin nasal cream (Alliance Pharmaceuticals Ltd) take 0.5 application four times a day Into each nostril</t>
+          <t>Naseptin nasal cream (Alliance Pharmaceuticals Ltd) take application four times a day Into each nostril</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Acidex liquid aniseed (Pinewood Healthcare) take 0.025 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Acidex liquid aniseed (Pinewood Healthcare) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Acidex liquid aniseed (Pinewood Healthcare) take 0.05 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Acidex liquid aniseed (Pinewood Healthcare) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Acidex liquid peppermint (Pinewood Healthcare) take 0.025 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Acidex liquid peppermint (Pinewood Healthcare) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Acidex liquid peppermint (Pinewood Healthcare) take 0.05 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Acidex liquid peppermint (Pinewood Healthcare) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5921,7 +5921,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>Gastrocote chewable tablets (Actavis UK Ltd) take 0.02 tablets four times a day for indigestion after meals and at bedtime</t>
+          <t>Gastrocote chewable tablets (Actavis UK Ltd) take tablets four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>Gastrocote chewable tablets (Actavis UK Ltd) take 0.04 tablets four times a day for indigestion after meals and at bedtime</t>
+          <t>Gastrocote chewable tablets (Actavis UK Ltd) take tablets four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>Gastrocote liquid (Actavis UK Ltd) take 0.1 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Gastrocote liquid (Actavis UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>Gastrocote liquid (Actavis UK Ltd) take 0.2 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Gastrocote liquid (Actavis UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>Gastrocote liquid (Actavis UK Ltd) take 0.3 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Gastrocote liquid (Actavis UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -5996,7 +5996,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>Gaviscon Advance chewable tablets (Reckitt Benckiser Plc) take 0.02 tablets four times a day for indigestion after meals and at bedtime</t>
+          <t>Gaviscon Advance chewable tablets (Reckitt Benckiser Plc) take tablets four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>Gaviscon Advance chewable tablets (Reckitt Benckiser Plc) take 0.04 tablets four times a day for indigestion after meals and at bedtime</t>
+          <t>Gaviscon Advance chewable tablets (Reckitt Benckiser Plc) take tablets four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6386,7 +6386,7 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>Mucogel oral suspension (Forest Laboratories UK Ltd) take 0.05 gel four times a day for indigestion after meals and at bedtime</t>
+          <t>Mucogel oral suspension (Forest Laboratories UK Ltd) take gel four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>Mucogel oral suspension (Forest Laboratories UK Ltd) take 0.1 gel four times a day for indigestion after meals and at bedtime</t>
+          <t>Mucogel oral suspension (Forest Laboratories UK Ltd) take gel four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6956,7 +6956,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>Peptac liquid aniseed (Teva UK Ltd) take 10 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Peptac liquid aniseed (Teva UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6971,7 +6971,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>Peptac liquid aniseed (Teva UK Ltd) take 20 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Peptac liquid aniseed (Teva UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>Peptac liquid peppermint (Teva UK Ltd) take 10 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Peptac liquid peppermint (Teva UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -7001,7 +7001,7 @@
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>Peptac liquid peppermint (Teva UK Ltd) take 20 liquid four times a day for indigestion after meals and at bedtime</t>
+          <t>Peptac liquid peppermint (Teva UK Ltd) take liquid four times a day for indigestion after meals and at bedtime</t>
         </is>
       </c>
     </row>
@@ -8726,7 +8726,7 @@
       </c>
       <c r="C550" t="inlineStr">
         <is>
-          <t>Lacri-lube eye ointment (Allergan Ltd) apply 1 application to eye if necessary for dry eyes</t>
+          <t>Lacri-lube eye ointment (Allergan Ltd) apply application if necessary for dry eyes</t>
         </is>
       </c>
     </row>
@@ -8741,7 +8741,7 @@
       </c>
       <c r="C551" t="inlineStr">
         <is>
-          <t>Lubri-Tears eye ointment (Alcon Laboratories (UK) Ltd) apply 1 application to eye if necessary for dry eyes</t>
+          <t>Lubri-Tears eye ointment (Alcon Laboratories (UK) Ltd) apply application if necessary for dry eyes</t>
         </is>
       </c>
     </row>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>Simple eye ointment apply 2.5 application to eye if necessary for dry eyes</t>
+          <t>Simple eye ointment apply application if necessary for dry eyes</t>
         </is>
       </c>
     </row>
@@ -9101,7 +9101,7 @@
       </c>
       <c r="C575" t="inlineStr">
         <is>
-          <t>Artificial saliva spray take 10 spray if necessary for dry mouth</t>
+          <t>Artificial saliva spray take spray if necessary for dry mouth</t>
         </is>
       </c>
     </row>
@@ -9116,7 +9116,7 @@
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>Dioralyte oral powder sachets blackcurrant (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte oral powder sachets blackcurrant (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="C577" t="inlineStr">
         <is>
-          <t>Dioralyte oral powder sachets citrus (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte oral powder sachets citrus (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9146,7 +9146,7 @@
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>Dioralyte oral powder sachets plain (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte oral powder sachets plain (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9161,7 +9161,7 @@
       </c>
       <c r="C579" t="inlineStr">
         <is>
-          <t>Dioralyte Relief oral powder sachets apricot (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte Relief oral powder sachets apricot (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9176,7 +9176,7 @@
       </c>
       <c r="C580" t="inlineStr">
         <is>
-          <t>Dioralyte Relief oral powder sachets blackcurrant (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte Relief oral powder sachets blackcurrant (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9191,7 +9191,7 @@
       </c>
       <c r="C581" t="inlineStr">
         <is>
-          <t>Dioralyte Relief oral powder sachets raspberry (sanofi-aventis) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Dioralyte Relief oral powder sachets raspberry (sanofi-aventis) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9206,7 +9206,7 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>Electrolade oral powder sachets banana (Actavis UK Ltd) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Electrolade oral powder sachets banana (Actavis UK Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>Electrolade oral powder sachets blackcurrant (Actavis UK Ltd) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Electrolade oral powder sachets blackcurrant (Actavis UK Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9236,7 +9236,7 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Electrolade oral powder sachets lemon and lime (Actavis UK Ltd) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Electrolade oral powder sachets lemon and lime (Actavis UK Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>Electrolade oral powder sachets multiflavour (Actavis UK Ltd) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Electrolade oral powder sachets multiflavour (Actavis UK Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9266,7 +9266,7 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>Electrolade oral powder sachets orange (Actavis UK Ltd) take 5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Electrolade oral powder sachets orange (Actavis UK Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9356,7 +9356,7 @@
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>Rapolyte oral powder sachets blackcurrant (Galen Ltd) take 0.5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Rapolyte oral powder sachets blackcurrant (Galen Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9371,7 +9371,7 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>Rapolyte oral powder sachets raspberry (Galen Ltd) take 0.5 sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
+          <t>Rapolyte oral powder sachets raspberry (Galen Ltd) take sachets if necessary for diarrhoea Reconstitute with 200ml water</t>
         </is>
       </c>
     </row>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>Saliva replacement liquid take 1 liquid if necessary for dry mouth</t>
+          <t>Saliva replacement liquid take liquid if necessary for dry mouth</t>
         </is>
       </c>
     </row>
@@ -9401,7 +9401,7 @@
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>Saliva stimulating tablets take half a tablet if necessary for dry mouth</t>
+          <t>Saliva stimulating tablets take tablets if necessary for dry mouth</t>
         </is>
       </c>
     </row>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>Aqueous cream apply to skin 0.00166667 application if necessary for dry skin</t>
+          <t>Aqueous cream apply to skin application if necessary for dry skin</t>
         </is>
       </c>
     </row>
@@ -9536,7 +9536,7 @@
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>Dermol cream (Dermal Laboratories Ltd) apply to skin 0.002 application if necessary for dry skin</t>
+          <t>Dermol cream (Dermal Laboratories Ltd) apply to skin application if necessary for dry skin</t>
         </is>
       </c>
     </row>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="C610" t="inlineStr">
         <is>
-          <t>Emulsifying ointment apply to skin 0.0222222 application if necessary for dry skin</t>
+          <t>Emulsifying ointment apply to skin application if necessary for dry skin</t>
         </is>
       </c>
     </row>
@@ -9731,7 +9731,7 @@
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>Sudocrem antiseptic healing cream (Forest Laboratories UK Ltd) apply to skin 0.4 application if necessary for skin care</t>
+          <t>Sudocrem antiseptic healing cream (Forest Laboratories UK Ltd) apply to skin application if necessary for skin care</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>Zinc and Castor oil ointment apply to skin 0.2 application if necessary for skin care</t>
+          <t>Zinc and Castor oil ointment apply to skin application if necessary for skin care</t>
         </is>
       </c>
     </row>
@@ -9896,7 +9896,7 @@
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>Neo-Cortef ear/eye ointment (PLIVA Pharma Ltd) apply 0.0877193 application to ear once a day</t>
+          <t>Neo-Cortef ear/eye ointment (PLIVA Pharma Ltd) apply application once a day</t>
         </is>
       </c>
     </row>
@@ -10436,7 +10436,7 @@
       </c>
       <c r="C664" t="inlineStr">
         <is>
-          <t>Abidec Multivitamin drops (Chefaro UK Ltd) take 0.002 drops once a day</t>
+          <t>Abidec Multivitamin drops (Chefaro UK Ltd) take drops once a day</t>
         </is>
       </c>
     </row>
@@ -12986,7 +12986,7 @@
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>Calcium and Ergocalciferol tablets take 0.002 tablets once a day</t>
+          <t>Calcium and Ergocalciferol tablets take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -13001,7 +13001,7 @@
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>Calcium and Ergocalciferol tablets take 0.004 tablets once a day</t>
+          <t>Calcium and Ergocalciferol tablets take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -14756,7 +14756,7 @@
       </c>
       <c r="C952" t="inlineStr">
         <is>
-          <t>Dalivit oral drops (LPC Medical (UK) Ltd) take 0.012 drops once a day</t>
+          <t>Dalivit oral drops (LPC Medical (UK) Ltd) take drops once a day</t>
         </is>
       </c>
     </row>
@@ -19331,7 +19331,7 @@
       </c>
       <c r="C1257" t="inlineStr">
         <is>
-          <t>Ketovite liquid (Waymade Healthcare Plc) take 0.025 liquid once a day</t>
+          <t>Ketovite liquid (Waymade Healthcare Plc) take liquid once a day</t>
         </is>
       </c>
     </row>
@@ -22466,7 +22466,7 @@
       </c>
       <c r="C1466" t="inlineStr">
         <is>
-          <t>Omacor capsules (Solvay Healthcare Ltd) take 0.025 capsules once a day</t>
+          <t>Omacor capsules (Solvay Healthcare Ltd) take capsules once a day</t>
         </is>
       </c>
     </row>
@@ -22481,7 +22481,7 @@
       </c>
       <c r="C1467" t="inlineStr">
         <is>
-          <t>Omacor capsules (Solvay Healthcare Ltd) take 0.05 capsules once a day</t>
+          <t>Omacor capsules (Solvay Healthcare Ltd) take capsules once a day</t>
         </is>
       </c>
     </row>
@@ -22496,7 +22496,7 @@
       </c>
       <c r="C1468" t="inlineStr">
         <is>
-          <t>Omacor capsules (Solvay Healthcare Ltd) take 0.1 capsules once a day</t>
+          <t>Omacor capsules (Solvay Healthcare Ltd) take capsules once a day</t>
         </is>
       </c>
     </row>
@@ -24116,7 +24116,7 @@
       </c>
       <c r="C1576" t="inlineStr">
         <is>
-          <t>Premique Low Dose tablets (Wyeth Pharmaceuticals) take 0.8 tablets once a day</t>
+          <t>Premique Low Dose tablets (Wyeth Pharmaceuticals) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -24131,7 +24131,7 @@
       </c>
       <c r="C1577" t="inlineStr">
         <is>
-          <t>Premique tablets (Wyeth Pharmaceuticals) take 0.8 tablets once a day</t>
+          <t>Premique tablets (Wyeth Pharmaceuticals) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -25091,7 +25091,7 @@
       </c>
       <c r="C1641" t="inlineStr">
         <is>
-          <t>Rifater tablets (sanofi-aventis) take 0.01 tablets once a day</t>
+          <t>Rifater tablets (sanofi-aventis) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -25106,7 +25106,7 @@
       </c>
       <c r="C1642" t="inlineStr">
         <is>
-          <t>Rifater tablets (sanofi-aventis) take 0.0133333 tablets once a day</t>
+          <t>Rifater tablets (sanofi-aventis) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -25121,7 +25121,7 @@
       </c>
       <c r="C1643" t="inlineStr">
         <is>
-          <t>Rifater tablets (sanofi-aventis) take 0.0166667 tablets once a day</t>
+          <t>Rifater tablets (sanofi-aventis) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -25136,7 +25136,7 @@
       </c>
       <c r="C1644" t="inlineStr">
         <is>
-          <t>Rifater tablets (sanofi-aventis) take 0.02 tablets once a day</t>
+          <t>Rifater tablets (sanofi-aventis) take tablets once a day</t>
         </is>
       </c>
     </row>
@@ -28736,7 +28736,7 @@
       </c>
       <c r="C1884" t="inlineStr">
         <is>
-          <t>Ultraproct suppositories (Meadow Laboratories Ltd) insert in anus 0.05 suppositories once a day Insert after bowel movement</t>
+          <t>Ultraproct suppositories (Meadow Laboratories Ltd) insert in anus suppositories once a day Insert after bowel movement</t>
         </is>
       </c>
     </row>
@@ -30311,7 +30311,7 @@
       </c>
       <c r="C1989" t="inlineStr">
         <is>
-          <t>Nystaform HC cream (Typharm Ltd) apply to skin 0.25 application once a day</t>
+          <t>Nystaform HC cream (Typharm Ltd) apply to skin application once a day</t>
         </is>
       </c>
     </row>
@@ -30326,7 +30326,7 @@
       </c>
       <c r="C1990" t="inlineStr">
         <is>
-          <t>Nystaform HC ointment (Typharm Ltd) apply to skin 0.25 application once a day</t>
+          <t>Nystaform HC ointment (Typharm Ltd) apply to skin application once a day</t>
         </is>
       </c>
     </row>
@@ -30521,7 +30521,7 @@
       </c>
       <c r="C2003" t="inlineStr">
         <is>
-          <t>Timodine cream (Reckitt Benckiser Plc) apply to skin 1 application once a day</t>
+          <t>Timodine cream (Reckitt Benckiser Plc) apply to skin application once a day</t>
         </is>
       </c>
     </row>
@@ -30581,7 +30581,7 @@
       </c>
       <c r="C2007" t="inlineStr">
         <is>
-          <t>Trimovate cream (GlaxoSmithKline) apply to skin 40 application once a day</t>
+          <t>Trimovate cream (GlaxoSmithKline) apply to skin application once a day</t>
         </is>
       </c>
     </row>
@@ -37136,7 +37136,7 @@
       </c>
       <c r="C2444" t="inlineStr">
         <is>
-          <t>Picolax oral powder sachets (Ferring Pharmaceuticals Ltd) take 0.5 sachets once only Dissolve in 150ml of water before taking</t>
+          <t>Picolax oral powder sachets (Ferring Pharmaceuticals Ltd) take sachets once only Dissolve in 150ml of water before taking</t>
         </is>
       </c>
     </row>
@@ -38171,7 +38171,7 @@
       </c>
       <c r="C2513" t="inlineStr">
         <is>
-          <t>Otomize ear spray (Waymade Healthcare Plc) apply 1 spray to ear three times a day</t>
+          <t>Otomize ear spray (Waymade Healthcare Plc) apply spray three times a day</t>
         </is>
       </c>
     </row>
@@ -42101,7 +42101,7 @@
       </c>
       <c r="C2775" t="inlineStr">
         <is>
-          <t>Ketovite tablets (Waymade Healthcare Plc) take 0.0025 tablets three times a day</t>
+          <t>Ketovite tablets (Waymade Healthcare Plc) take tablets three times a day</t>
         </is>
       </c>
     </row>
@@ -43541,7 +43541,7 @@
       </c>
       <c r="C2871" t="inlineStr">
         <is>
-          <t>Pancrease HL gastro-resistant capsules (Janssen-Cilag Ltd) take 0.2 capsules three times a day with meals</t>
+          <t>Pancrease HL gastro-resistant capsules (Janssen-Cilag Ltd) take capsules three times a day with meals</t>
         </is>
       </c>
     </row>
@@ -43556,7 +43556,7 @@
       </c>
       <c r="C2872" t="inlineStr">
         <is>
-          <t>Pancrease HL gastro-resistant capsules (Janssen-Cilag Ltd) take 0.4 capsules three times a day with meals</t>
+          <t>Pancrease HL gastro-resistant capsules (Janssen-Cilag Ltd) take capsules three times a day with meals</t>
         </is>
       </c>
     </row>
@@ -43571,7 +43571,7 @@
       </c>
       <c r="C2873" t="inlineStr">
         <is>
-          <t>Pancrex gastro-resistant granules (Paines &amp; Byrne Ltd) take 1 granule three times a day with meals</t>
+          <t>Pancrex gastro-resistant granules (Paines &amp; Byrne Ltd) take granules three times a day with meals</t>
         </is>
       </c>
     </row>
@@ -43586,7 +43586,7 @@
       </c>
       <c r="C2874" t="inlineStr">
         <is>
-          <t>Pancrex gastro-resistant granules (Paines &amp; Byrne Ltd) take 2 granules three times a day with meals</t>
+          <t>Pancrex gastro-resistant granules (Paines &amp; Byrne Ltd) take granules three times a day with meals</t>
         </is>
       </c>
     </row>
@@ -43916,7 +43916,7 @@
       </c>
       <c r="C2896" t="inlineStr">
         <is>
-          <t>Phosphate Sandoz effervescent tablets (HK Pharma Ltd) take half a tablet three times a day</t>
+          <t>Phosphate Sandoz effervescent tablets (HK Pharma Ltd) take tablets three times a day</t>
         </is>
       </c>
     </row>
@@ -46571,7 +46571,7 @@
       </c>
       <c r="C3073" t="inlineStr">
         <is>
-          <t>Tinaderm-M cream (Schering-Plough Ltd) apply to skin 0.5 application three times a day</t>
+          <t>Tinaderm-M cream (Schering-Plough Ltd) apply to skin application three times a day</t>
         </is>
       </c>
     </row>
@@ -46706,7 +46706,7 @@
       </c>
       <c r="C3082" t="inlineStr">
         <is>
-          <t>Neo-Cortef ear/eye ointment (PLIVA Pharma Ltd) apply 1 application to ear twice a day</t>
+          <t>Neo-Cortef ear/eye ointment (PLIVA Pharma Ltd) apply application twice a day</t>
         </is>
       </c>
     </row>
@@ -49001,7 +49001,7 @@
       </c>
       <c r="C3235" t="inlineStr">
         <is>
-          <t>Naseptin nasal cream (Alliance Pharmaceuticals Ltd) take 5 application twice a day Into each nostril</t>
+          <t>Naseptin nasal cream (Alliance Pharmaceuticals Ltd) take application twice a day Into each nostril</t>
         </is>
       </c>
     </row>
@@ -58826,7 +58826,7 @@
       </c>
       <c r="C3890" t="inlineStr">
         <is>
-          <t>Phosphate Sandoz effervescent tablets (HK Pharma Ltd) take 0.008 tablets twice a day</t>
+          <t>Phosphate Sandoz effervescent tablets (HK Pharma Ltd) take tablets twice a day</t>
         </is>
       </c>
     </row>
@@ -62891,7 +62891,7 @@
       </c>
       <c r="C4161" t="inlineStr">
         <is>
-          <t>Trizivir tablets (GlaxoSmithKline) take 0.02 tablets twice a day</t>
+          <t>Trizivir tablets (GlaxoSmithKline) take tablets twice a day</t>
         </is>
       </c>
     </row>
@@ -63911,7 +63911,7 @@
       </c>
       <c r="C4229" t="inlineStr">
         <is>
-          <t>Anugesic-HC suppositories (Pfizer Ltd) insert in anus 10 suppositories twice a day Insert after bowel movement</t>
+          <t>Anugesic-HC suppositories (Pfizer Ltd) insert in anus suppositories twice a day Insert after bowel movement</t>
         </is>
       </c>
     </row>
@@ -63926,7 +63926,7 @@
       </c>
       <c r="C4230" t="inlineStr">
         <is>
-          <t>Anusol HC suppositories (McNeil Ltd) insert in anus 10 suppositories twice a day Insert after bowel movement</t>
+          <t>Anusol HC suppositories (McNeil Ltd) insert in anus suppositories twice a day Insert after bowel movement</t>
         </is>
       </c>
     </row>
@@ -64241,7 +64241,7 @@
       </c>
       <c r="C4251" t="inlineStr">
         <is>
-          <t>Anugesic-HC cream (Pfizer Ltd) apply to skin 20 application twice a day Apply after bowel movement</t>
+          <t>Anugesic-HC cream (Pfizer Ltd) apply to skin application twice a day Apply after bowel movement</t>
         </is>
       </c>
     </row>
@@ -64256,7 +64256,7 @@
       </c>
       <c r="C4252" t="inlineStr">
         <is>
-          <t>Anusol HC ointment (McNeil Ltd) apply to skin 20 application twice a day Apply after bowel movement</t>
+          <t>Anusol HC ointment (McNeil Ltd) apply to skin application twice a day Apply after bowel movement</t>
         </is>
       </c>
     </row>
@@ -64301,7 +64301,7 @@
       </c>
       <c r="C4255" t="inlineStr">
         <is>
-          <t>Benzoic acid compound ointment apply to skin 0.05 application twice a day</t>
+          <t>Benzoic acid compound ointment apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -65996,7 +65996,7 @@
       </c>
       <c r="C4368" t="inlineStr">
         <is>
-          <t>Nystaform HC cream (Typharm Ltd) apply to skin 0.25 application twice a day</t>
+          <t>Nystaform HC cream (Typharm Ltd) apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -66011,7 +66011,7 @@
       </c>
       <c r="C4369" t="inlineStr">
         <is>
-          <t>Nystaform HC ointment (Typharm Ltd) apply to skin 0.25 application twice a day</t>
+          <t>Nystaform HC ointment (Typharm Ltd) apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -66251,7 +66251,7 @@
       </c>
       <c r="C4385" t="inlineStr">
         <is>
-          <t>Timodine cream (Reckitt Benckiser Plc) apply to skin 1 application twice a day</t>
+          <t>Timodine cream (Reckitt Benckiser Plc) apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -66266,7 +66266,7 @@
       </c>
       <c r="C4386" t="inlineStr">
         <is>
-          <t>Tinaderm-M cream (Schering-Plough Ltd) apply to skin 1 application twice a day</t>
+          <t>Tinaderm-M cream (Schering-Plough Ltd) apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -66341,7 +66341,7 @@
       </c>
       <c r="C4391" t="inlineStr">
         <is>
-          <t>Trimovate cream (GlaxoSmithKline) apply to skin 40 application twice a day</t>
+          <t>Trimovate cream (GlaxoSmithKline) apply to skin application twice a day</t>
         </is>
       </c>
     </row>
@@ -66356,7 +66356,7 @@
       </c>
       <c r="C4392" t="inlineStr">
         <is>
-          <t>Ultraproct ointment (Meadow Laboratories Ltd) apply to skin 40 application twice a day Apply after bowel movement</t>
+          <t>Ultraproct ointment (Meadow Laboratories Ltd) apply to skin application twice a day Apply after bowel movement</t>
         </is>
       </c>
     </row>

</xml_diff>